<commit_message>
Added ETD44 work in progress
</commit_message>
<xml_diff>
--- a/Inductor_Design_Selection_Worksheet.xlsx
+++ b/Inductor_Design_Selection_Worksheet.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott.mcelroy\Desktop\Personal\InductorDesign\inductor_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563DDCCA-E256-4721-BDAF-D6A25589A040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475F4421-9FB4-476C-88CC-38CA91BDBBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{880F8341-2F0F-419A-8A65-B6E7E097180D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{880F8341-2F0F-419A-8A65-B6E7E097180D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inductor Design Selector" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>Inductor Design Calculator</t>
   </si>
@@ -148,6 +159,81 @@
   </si>
   <si>
     <t>mm^4</t>
+  </si>
+  <si>
+    <t>Ferrite Core</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>ETD44</t>
+  </si>
+  <si>
+    <t>Magnetic Path Length (MPL)</t>
+  </si>
+  <si>
+    <t>Mean Length per Turn (MLT)</t>
+  </si>
+  <si>
+    <t>Core Weight (Wfte)</t>
+  </si>
+  <si>
+    <t>Cross Sectional Area (Ac)</t>
+  </si>
+  <si>
+    <t>Window Area (Wa)</t>
+  </si>
+  <si>
+    <t>Surface Area (At)</t>
+  </si>
+  <si>
+    <t>Permeability (Urc)</t>
+  </si>
+  <si>
+    <t>Core Dimensions</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Center Post Diameter</t>
+  </si>
+  <si>
+    <t>Center Post Radius</t>
+  </si>
+  <si>
+    <t>mm^2</t>
+  </si>
+  <si>
+    <t>Window Width</t>
+  </si>
+  <si>
+    <t>Window Height</t>
+  </si>
+  <si>
+    <t>Outer wall to outer wall width</t>
+  </si>
+  <si>
+    <t>Effective Volume</t>
+  </si>
+  <si>
+    <t>mm^3</t>
+  </si>
+  <si>
+    <t>Effective Cross Section (Ae)</t>
+  </si>
+  <si>
+    <t>Area Product (Ap) accounting for Ku</t>
   </si>
 </sst>
 </file>
@@ -197,12 +283,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -226,14 +318,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,6 +329,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,337 +653,513 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37D8677-D162-484C-A08B-46DF1FF04C8F}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.19921875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>170</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="4">
+        <v>115.35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>30</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="4">
+        <v>55</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
-        <v>50</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <f>B7*B6</f>
-        <v>1500</v>
-      </c>
-      <c r="C8" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4">
+        <f>PI()*F21^2</f>
+        <v>181.45839167134645</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>0.95</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="3"/>
+      <c r="E9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="4">
+        <v>173</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <f>B8/B9</f>
-        <v>1578.9473684210527</v>
-      </c>
-      <c r="C10" s="5" t="s">
+        <v>473.68421052631584</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="4">
+        <f>F23*F24</f>
+        <v>557.06000000000006</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <f>B10/B5</f>
-        <v>9.2879256965944279</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>2.7863777089783284</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+      <c r="E11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="10">
+        <f>F10*F9*B27</f>
+        <v>38548.552000000003</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>100000</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
+      <c r="E12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <f>B6/B5</f>
         <v>0.17647058823529413</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="3"/>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="4">
+        <v>124</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <f>1/B12</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="3"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
+      <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="4">
+        <v>17800</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
+      <c r="C16" s="3"/>
+      <c r="E16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <f>B7</f>
-        <v>50</v>
-      </c>
-      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="4">
+        <v>43.8</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>0.3</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="4">
+        <v>15.2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <f>B17*B18</f>
-        <v>15</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <v>4.5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
+      <c r="E19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="4">
+        <f>2*15.2</f>
+        <v>30.4</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <f>B17+B19</f>
-        <v>65</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>19.5</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="4">
+        <v>15.2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <f>((B5-B6)*B13)/(2*B19*B12)</f>
-        <v>8.2352941176470598E-6</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>2.7450980392156865E-5</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="3"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
+      <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="4">
+        <f>F20/2</f>
+        <v>7.6</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B23">
         <v>0.25</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="3" t="s">
+      <c r="E23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="4">
+        <f>F22-F20</f>
+        <v>17.3</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B24">
         <f>3*10^6</f>
         <v>3000000</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
+      <c r="E24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="4">
+        <f>16.1*2</f>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B25">
         <f>B24/1000000</f>
         <v>3</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="3" t="s">
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B26">
         <f>0.5*B21*B20^2</f>
-        <v>1.7397058823529415E-2</v>
-      </c>
-      <c r="C26" s="5" t="s">
+        <v>5.2191176470588237E-3</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B27">
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B28">
         <f>2*B26/(B27*B23*B24)</f>
-        <v>1.1598039215686276E-7</v>
-      </c>
-      <c r="C28" s="5" t="s">
+        <v>3.4794117647058826E-8</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="11">
         <f>B28*10^12</f>
-        <v>115980.39215686276</v>
-      </c>
-      <c r="C29" s="5" t="s">
+        <v>34794.117647058825</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" s="8">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <f>(2*3.45*10^-3)/(0.4*0.25*(3*10^6))</f>
         <v>2.3000000000000004E-8</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" s="7">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <f>A33*1000000000000</f>
         <v>23000.000000000004</v>
       </c>

</xml_diff>

<commit_message>
Added guess and check section
</commit_message>
<xml_diff>
--- a/Inductor_Design_Selection_Worksheet.xlsx
+++ b/Inductor_Design_Selection_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott.mcelroy\Desktop\Personal\InductorDesign\inductor_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC190C09-54E2-4B33-98DA-FADD2ADD8C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7D80F-41B4-4EA1-B17D-6A439DF8D54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{880F8341-2F0F-419A-8A65-B6E7E097180D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="135">
   <si>
     <t>Inductor Design Calculator</t>
   </si>
@@ -618,6 +618,63 @@
   </si>
   <si>
     <t>Wire diameter is completely based on current</t>
+  </si>
+  <si>
+    <t>Guess and check method</t>
+  </si>
+  <si>
+    <t>Core Area (Ac)</t>
+  </si>
+  <si>
+    <t>Core selected</t>
+  </si>
+  <si>
+    <t>ETD-44</t>
+  </si>
+  <si>
+    <t>gap (lg)</t>
+  </si>
+  <si>
+    <t>Turns (N)</t>
+  </si>
+  <si>
+    <t>Inductance (from gap)</t>
+  </si>
+  <si>
+    <t>Inductance (from gap and permeability)</t>
+  </si>
+  <si>
+    <t>effective permeability (ue)</t>
+  </si>
+  <si>
+    <t>effective permeability from gap (ue_gap)</t>
+  </si>
+  <si>
+    <t>Flux Density (Bdc) - using lg and um</t>
+  </si>
+  <si>
+    <t>Flux Density (Bdc) - using ue</t>
+  </si>
+  <si>
+    <t>Gap Needed with selected core and Bsat</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Saturation Flux Density</t>
+  </si>
+  <si>
+    <t>Winding Length</t>
+  </si>
+  <si>
+    <t>Fringing Factor</t>
+  </si>
+  <si>
+    <t>Inductance (from gap plus fringe)</t>
+  </si>
+  <si>
+    <t>Inductance (from gap and permeability and fringe)</t>
   </si>
 </sst>
 </file>
@@ -811,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -852,17 +909,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37D8677-D162-484C-A08B-46DF1FF04C8F}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,28 +1258,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1759,7 +1822,7 @@
       <c r="A21" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="39">
         <f>((B5-B6)*B13)/(2*B19*B12)</f>
         <v>2.4705882352941178E-5</v>
       </c>
@@ -1785,7 +1848,7 @@
       <c r="A22" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22" s="39">
         <f>B21</f>
         <v>2.4705882352941178E-5</v>
       </c>
@@ -1890,8 +1953,8 @@
         <v>31</v>
       </c>
       <c r="B26" s="10">
-        <f>6*10^6</f>
-        <v>6000000</v>
+        <f>8*10^6</f>
+        <v>8000000</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>30</v>
@@ -1919,7 +1982,7 @@
       </c>
       <c r="B27" s="10">
         <f>B26/10000</f>
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>77</v>
@@ -1953,7 +2016,7 @@
       </c>
       <c r="B28" s="10">
         <f>B26/1000000</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>33</v>
@@ -1983,7 +2046,7 @@
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="38">
         <f>0.5*B21*B20^2</f>
         <v>3.7367647058823533E-2</v>
       </c>
@@ -2026,7 +2089,7 @@
       </c>
       <c r="B31" s="10">
         <f>2*B29/(B30*B25*B26)</f>
-        <v>1.4154411764705883E-7</v>
+        <v>1.0615808823529411E-7</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>34</v>
@@ -2044,7 +2107,7 @@
       </c>
       <c r="B32" s="10">
         <f>B31*100000000</f>
-        <v>14.154411764705884</v>
+        <v>10.615808823529411</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>71</v>
@@ -2066,7 +2129,7 @@
       </c>
       <c r="B33" s="10">
         <f>B31*10^12</f>
-        <v>141544.11764705883</v>
+        <v>106158.08823529411</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>35</v>
@@ -2212,7 +2275,7 @@
       </c>
       <c r="B41" s="26">
         <f>(2*B29*10^4)/(B25*B27*B30)</f>
-        <v>14.154411764705882</v>
+        <v>10.615808823529411</v>
       </c>
       <c r="C41" s="21" t="s">
         <v>71</v>
@@ -2230,7 +2293,7 @@
       </c>
       <c r="B42" s="26">
         <f>B41*10000</f>
-        <v>141544.11764705883</v>
+        <v>106158.08823529411</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>35</v>
@@ -2240,7 +2303,7 @@
       </c>
       <c r="F42" s="29">
         <f>B23/B27</f>
-        <v>8.3472106673981764E-2</v>
+        <v>6.2604080005486326E-2</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>79</v>
@@ -2254,7 +2317,7 @@
       </c>
       <c r="F43" s="29">
         <f>F42*100</f>
-        <v>8.3472106673981763</v>
+        <v>6.2604080005486322</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>52</v>
@@ -2268,7 +2331,7 @@
       <c r="E44" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="F44" s="29">
+      <c r="F44" s="26">
         <v>0.08</v>
       </c>
       <c r="G44" s="30" t="s">
@@ -2287,7 +2350,7 @@
       </c>
       <c r="F45" s="29">
         <f>F43/F44</f>
-        <v>104.3401333424772</v>
+        <v>78.255100006857901</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>91</v>
@@ -2303,7 +2366,7 @@
       </c>
       <c r="F46" s="29">
         <f>ROUND(F45,0)</f>
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>91</v>
@@ -2319,7 +2382,7 @@
       </c>
       <c r="F47" s="29">
         <f>F46*F44</f>
-        <v>8.32</v>
+        <v>6.24</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>52</v>
@@ -2335,14 +2398,14 @@
       </c>
       <c r="F48" s="29">
         <f>0.1*F47</f>
-        <v>0.83200000000000007</v>
+        <v>0.62400000000000011</v>
       </c>
       <c r="G48" s="30" t="s">
         <v>79</v>
       </c>
       <c r="H48" s="27"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E49" s="28" t="s">
         <v>97</v>
       </c>
@@ -2354,7 +2417,7 @@
       </c>
       <c r="H49" s="27"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>80</v>
       </c>
@@ -2371,26 +2434,26 @@
       </c>
       <c r="H50" s="27"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
       <c r="B52">
         <v>0.6</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -2398,15 +2461,202 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="4">
+        <f>F11</f>
+        <v>1.742</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2.9750000000000001</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="4">
+        <f>(1+(B61/SQRT(B59))*LN(2*B62/B61))</f>
+        <v>1.3095791968836514</v>
+      </c>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="46">
+        <f>(0.4*PI()*B60^2*B59*(10^-8))/B61</f>
+        <v>9.6537623661042325E-5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="46">
+        <f>(0.4*PI()*B60^2*F11*(10^-8))/(B61+(F6/F22))</f>
+        <v>9.0865418734010172E-5</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="45">
+        <f>B64*B63</f>
+        <v>1.2642366366308401E-4</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="45">
+        <f>B63*B65</f>
+        <v>1.1899546209018173E-4</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="4">
+        <f>F22/(1+F22*(B61/F6))</f>
+        <v>96.948088990302338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B69" s="4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B70" s="4">
+        <f>(B69*(0.4*PI()*B60*B7)/F6)/10000</f>
+        <v>1.5884868485335575</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="44">
+        <f>(0.4*PI()*B60*B7)/(B61+(F6/F22))/10000</f>
+        <v>1.2419416479964214</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="4">
+        <f>(0.4*PI()*B60*B7*(10^-4)/(B25*10000))</f>
+        <v>5.9975859750350598E-5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="44">
+        <f>(0.4*PI()*B60*(B7+B19)*(10^-4))/(B61+(F6/F22))</f>
+        <v>1.3661358127960634</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="E52:H52"/>
+    <mergeCell ref="A57:I57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added total core power loss
</commit_message>
<xml_diff>
--- a/Inductor_Design_Selection_Worksheet.xlsx
+++ b/Inductor_Design_Selection_Worksheet.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott.mcelroy\Desktop\Personal\InductorDesign\inductor_design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\OneDrive\Desktop\Projects\InductorDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7D80F-41B4-4EA1-B17D-6A439DF8D54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468F5F31-4C8A-4939-B359-437FC5D21DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{880F8341-2F0F-419A-8A65-B6E7E097180D}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="10425" windowHeight="13043" xr2:uid="{880F8341-2F0F-419A-8A65-B6E7E097180D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inductor Design Selector" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="146">
   <si>
     <t>Inductor Design Calculator</t>
   </si>
@@ -662,9 +651,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>Saturation Flux Density</t>
-  </si>
-  <si>
     <t>Winding Length</t>
   </si>
   <si>
@@ -675,6 +661,42 @@
   </si>
   <si>
     <t>Inductance (from gap and permeability and fringe)</t>
+  </si>
+  <si>
+    <t>Hac_max</t>
+  </si>
+  <si>
+    <t>A*T/cm</t>
+  </si>
+  <si>
+    <t>Bac_max</t>
+  </si>
+  <si>
+    <t>Hac_min</t>
+  </si>
+  <si>
+    <t>Bac_min</t>
+  </si>
+  <si>
+    <t>Bac/2 (for loss curve)</t>
+  </si>
+  <si>
+    <t>Saturation Flux Density (for saturation)</t>
+  </si>
+  <si>
+    <t>Power Loss based on graph</t>
+  </si>
+  <si>
+    <t>mW</t>
+  </si>
+  <si>
+    <t>mW/cm^3</t>
+  </si>
+  <si>
+    <t>Core Power Loss (W)</t>
+  </si>
+  <si>
+    <t>Core Power Loss (mW)</t>
   </si>
 </sst>
 </file>
@@ -868,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -911,6 +933,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,9 +947,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,48 +1261,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37D8677-D162-484C-A08B-46DF1FF04C8F}">
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>75</v>
       </c>
@@ -1300,7 +1321,7 @@
       <c r="L3" s="31"/>
       <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1329,7 +1350,7 @@
       </c>
       <c r="M4" s="27"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1361,7 +1382,7 @@
       </c>
       <c r="M5" s="27"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1413,7 @@
       </c>
       <c r="M6" s="27"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1424,7 +1445,7 @@
       </c>
       <c r="M7" s="27"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1477,7 @@
       </c>
       <c r="M8" s="27"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -1485,7 +1506,7 @@
       </c>
       <c r="M9" s="27"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1518,7 +1539,7 @@
       </c>
       <c r="M10" s="27"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1550,7 +1571,7 @@
       </c>
       <c r="M11" s="27"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1579,7 +1600,7 @@
       </c>
       <c r="M12" s="27"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -1607,7 +1628,7 @@
       </c>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -1640,7 +1661,7 @@
       </c>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="6"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -1665,7 +1686,7 @@
       </c>
       <c r="M15" s="27"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="23" t="s">
         <v>13</v>
       </c>
@@ -1690,7 +1711,7 @@
       </c>
       <c r="M16" s="27"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1721,7 +1742,7 @@
       </c>
       <c r="M17" s="27"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -1752,7 +1773,7 @@
       </c>
       <c r="M18" s="27"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
@@ -1786,7 +1807,7 @@
       </c>
       <c r="M19" s="27"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1818,7 +1839,7 @@
       </c>
       <c r="M20" s="27"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>110</v>
       </c>
@@ -1844,7 +1865,7 @@
       <c r="L21" s="30"/>
       <c r="M21" s="27"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>111</v>
       </c>
@@ -1870,7 +1891,7 @@
       <c r="L22" s="30"/>
       <c r="M22" s="27"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>59</v>
       </c>
@@ -1898,7 +1919,7 @@
       <c r="L23" s="30"/>
       <c r="M23" s="27"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
         <v>76</v>
       </c>
@@ -1921,7 +1942,7 @@
       </c>
       <c r="M24" s="27"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>28</v>
       </c>
@@ -1948,7 +1969,7 @@
       </c>
       <c r="M25" s="27"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -1976,7 +1997,7 @@
       </c>
       <c r="M26" s="27"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -2010,7 +2031,7 @@
       </c>
       <c r="M27" s="27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>32</v>
       </c>
@@ -2042,7 +2063,7 @@
       </c>
       <c r="M28" s="27"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -2070,7 +2091,7 @@
       </c>
       <c r="M29" s="27"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>26</v>
       </c>
@@ -2083,7 +2104,7 @@
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
@@ -2101,7 +2122,7 @@
       <c r="G31" s="25"/>
       <c r="H31" s="31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>27</v>
       </c>
@@ -2123,7 +2144,7 @@
       </c>
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>27</v>
       </c>
@@ -2145,7 +2166,7 @@
       </c>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B34" s="4"/>
       <c r="E34" s="28" t="s">
         <v>48</v>
@@ -2159,7 +2180,7 @@
       </c>
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="23" t="s">
         <v>78</v>
       </c>
@@ -2176,7 +2197,7 @@
       </c>
       <c r="H35" s="27"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="20" t="s">
         <v>64</v>
       </c>
@@ -2197,7 +2218,7 @@
       </c>
       <c r="H36" s="27"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="20" t="s">
         <v>66</v>
       </c>
@@ -2219,7 +2240,7 @@
       </c>
       <c r="H37" s="27"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>67</v>
       </c>
@@ -2242,7 +2263,7 @@
       </c>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -2258,7 +2279,7 @@
       </c>
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="23" t="s">
         <v>74</v>
       </c>
@@ -2269,7 +2290,7 @@
       <c r="G40" s="30"/>
       <c r="H40" s="27"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="22" t="s">
         <v>72</v>
       </c>
@@ -2287,7 +2308,7 @@
       <c r="G41" s="31"/>
       <c r="H41" s="31"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="22" t="s">
         <v>73</v>
       </c>
@@ -2310,7 +2331,7 @@
       </c>
       <c r="H42" s="27"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="E43" s="28" t="s">
         <v>87</v>
@@ -2324,7 +2345,7 @@
       </c>
       <c r="H43" s="27"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>105</v>
       </c>
@@ -2341,7 +2362,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>106</v>
       </c>
@@ -2357,7 +2378,7 @@
       </c>
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>107</v>
       </c>
@@ -2373,7 +2394,7 @@
       </c>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>108</v>
       </c>
@@ -2389,7 +2410,7 @@
       </c>
       <c r="H47" s="27"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>109</v>
       </c>
@@ -2405,7 +2426,7 @@
       </c>
       <c r="H48" s="27"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E49" s="28" t="s">
         <v>97</v>
       </c>
@@ -2417,7 +2438,7 @@
       </c>
       <c r="H49" s="27"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="32" t="s">
         <v>80</v>
       </c>
@@ -2434,26 +2455,26 @@
       </c>
       <c r="H50" s="27"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>82</v>
       </c>
       <c r="B52">
         <v>0.6</v>
       </c>
-      <c r="E52" s="42" t="s">
+      <c r="E52" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -2461,25 +2482,25 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="45"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>118</v>
       </c>
@@ -2487,7 +2508,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>117</v>
       </c>
@@ -2499,7 +2520,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>121</v>
       </c>
@@ -2507,7 +2528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>120</v>
       </c>
@@ -2518,9 +2539,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="4">
         <v>2.9750000000000001</v>
@@ -2529,9 +2550,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="4">
         <f>(1+(B61/SQRT(B59))*LN(2*B62/B61))</f>
@@ -2539,11 +2560,11 @@
       </c>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B64" s="46">
+      <c r="B64" s="4">
         <f>(0.4*PI()*B60^2*B59*(10^-8))/B61</f>
         <v>9.6537623661042325E-5</v>
       </c>
@@ -2551,11 +2572,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="46">
+      <c r="B65" s="4">
         <f>(0.4*PI()*B60^2*F11*(10^-8))/(B61+(F6/F22))</f>
         <v>9.0865418734010172E-5</v>
       </c>
@@ -2563,11 +2584,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="45">
+        <v>132</v>
+      </c>
+      <c r="B66" s="41">
         <f>B64*B63</f>
         <v>1.2642366366308401E-4</v>
       </c>
@@ -2575,11 +2596,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B67" s="45">
+        <v>133</v>
+      </c>
+      <c r="B67" s="41">
         <f>B63*B65</f>
         <v>1.1899546209018173E-4</v>
       </c>
@@ -2587,7 +2608,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>124</v>
       </c>
@@ -2596,31 +2617,31 @@
         <v>96.948088990302338</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B69" s="4">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B70" s="4">
         <f>(B69*(0.4*PI()*B60*B7)/F6)/10000</f>
-        <v>1.5884868485335575</v>
+        <v>0.12810377810754497</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="44">
+      <c r="B71" s="40">
         <f>(0.4*PI()*B60*B7)/(B61+(F6/F22))/10000</f>
         <v>1.2419416479964214</v>
       </c>
@@ -2628,7 +2649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>128</v>
       </c>
@@ -2640,16 +2661,111 @@
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B73" s="44">
+        <v>140</v>
+      </c>
+      <c r="B73" s="40">
         <f>(0.4*PI()*B60*(B7+B19)*(10^-4))/(B61+(F6/F22))</f>
         <v>1.3661358127960634</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74">
+        <f>(B60/F6)*(B7+B19)</f>
+        <v>112.13592233009709</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75">
+        <f>B74*B69/10000</f>
+        <v>0.11213592233009709</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B76">
+        <f>(B60/F6)*(B7-B19)</f>
+        <v>91.747572815533985</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B77">
+        <f>B76*B69/10000</f>
+        <v>9.1747572815533987E-2</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78">
+        <f>(B75-B77)/2</f>
+        <v>1.019417475728155E-2</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79">
+        <v>300</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80">
+        <f>B79*F6*B59</f>
+        <v>5382.78</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81">
+        <f>B80/1000</f>
+        <v>5.3827799999999995</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>